<commit_message>
brute force working for positive Y, need to add extra boundary checking for negative Y
</commit_message>
<xml_diff>
--- a/Day17_part2/part2_example.xlsx
+++ b/Day17_part2/part2_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bca5ddf6c3ac7bf9/Documents/GitHub/AoC2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bca5ddf6c3ac7bf9/Documents/GitHub/AoC2021/Day17_part2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4630B505-E9B6-4BD5-8919-49063B9DBB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{4630B505-E9B6-4BD5-8919-49063B9DBB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A009B2-6170-44B0-B04C-3907BB2C2508}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{4252A3F5-AC70-40CB-97BB-72CA01D71F48}"/>
+    <workbookView xWindow="15375" yWindow="1935" windowWidth="16920" windowHeight="16170" xr2:uid="{4252A3F5-AC70-40CB-97BB-72CA01D71F48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,95 +380,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35C92FD-86C5-4471-8AD2-4ABA4B140631}">
-  <dimension ref="B1:C114"/>
+  <dimension ref="B1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B94" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>6</v>
       </c>
       <c r="C1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>7</v>
       </c>
@@ -480,87 +506,117 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>7</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>7</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>7</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>7</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>7</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>7</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>7</v>
       </c>
       <c r="C19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>7</v>
       </c>
       <c r="C21">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>8</v>
       </c>
@@ -568,7 +624,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>8</v>
       </c>
@@ -576,23 +632,29 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>8</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>8</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>9</v>
       </c>
@@ -600,7 +662,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>9</v>
       </c>
@@ -608,23 +670,30 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>9</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>10</v>
       </c>
       <c r="C29">
         <v>-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f>SUM(E1:E28)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>10</v>
       </c>
@@ -632,7 +701,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>11</v>
       </c>
@@ -640,7 +709,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>11</v>
       </c>

</xml_diff>